<commit_message>
Cambios en la columna a estado por completada?
</commit_message>
<xml_diff>
--- a/api/public/templates/reporte-tareas.xlsx
+++ b/api/public/templates/reporte-tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Archivos\Documentos\GitHub\AppTareas\api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762986B1-EFFA-4BE5-9619-149B60D0132A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D000A3B2-BC83-40FF-A009-3F873B41E519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Prioridad</t>
   </si>
   <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>${table:tareas.nombre}</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>${descripcion}</t>
+  </si>
+  <si>
+    <t>¿Terminada?</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -558,30 +558,30 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio en columna de reporte (#6)
* Plantilla de reporte de excel

Se integro el archivo de plantilla de excel que se elimino por accidente.

* Mejora en el guardado de fechas

Se modifico la utileria y el guardado de la fecha para que sea UTC.

* Cambios en la columna a estado por completada?
</commit_message>
<xml_diff>
--- a/api/public/templates/reporte-tareas.xlsx
+++ b/api/public/templates/reporte-tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Archivos\Documentos\GitHub\AppTareas\api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762986B1-EFFA-4BE5-9619-149B60D0132A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D000A3B2-BC83-40FF-A009-3F873B41E519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Prioridad</t>
   </si>
   <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>${table:tareas.nombre}</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>${descripcion}</t>
+  </si>
+  <si>
+    <t>¿Terminada?</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -558,30 +558,30 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integra la generación de informes de Excel y optimiza las tareas.
Se ha añadido ExcelService para generar informes de forma eficiente utilizando ExcelJS y procesamiento por lotes asíncrono. Se ha actualizado la entidad tareas con índices para mejorar el rendimiento de las consultas. Se ha refactorizado el controlador y el servicio de tareas para mejorar la paginación y el orden. Se ha sustituido la lógica de plantillas XLSX heredada por un nuevo flujo de trabajo de informes de Excel en el trabajador. Se han actualizado las dependencias para incluir bull y @nestjs/bull para el futuro procesamiento de colas.
</commit_message>
<xml_diff>
--- a/api/public/templates/reporte-tareas.xlsx
+++ b/api/public/templates/reporte-tareas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Archivos\Documentos\GitHub\AppTareas\api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D000A3B2-BC83-40FF-A009-3F873B41E519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86DA69B-039E-4769-AFD8-184F2011828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Reporte de tareas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Reporte de tareas'!$A$4:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Reporte de tareas'!$A$4:$H$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>TODOLIST</t>
   </si>
@@ -54,31 +54,10 @@
     <t>Prioridad</t>
   </si>
   <si>
-    <t>${table:tareas.nombre}</t>
-  </si>
-  <si>
-    <t>${table:tareas.created}</t>
-  </si>
-  <si>
-    <t>${table:tareas.fecha_inicio}</t>
-  </si>
-  <si>
-    <t>${table:tareas.fecha_fin}</t>
-  </si>
-  <si>
-    <t>${table:tareas.fecha_terminado}</t>
-  </si>
-  <si>
-    <t>${table:tareas.prioridad}</t>
-  </si>
-  <si>
-    <t>${table:tareas.completado}</t>
-  </si>
-  <si>
-    <t>${descripcion}</t>
-  </si>
-  <si>
     <t>¿Terminada?</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
   </si>
 </sst>
 </file>
@@ -120,18 +99,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -152,21 +125,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +477,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,69 +494,57 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
+      <c r="H4" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:G4" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>